<commit_message>
UseCase Diagram & Scenario
</commit_message>
<xml_diff>
--- a/Scenario/Scenario-Glavni tok(Gost).xlsx
+++ b/Scenario/Scenario-Glavni tok(Gost).xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>GOST/UPOSLENIK USTANOVE</t>
   </si>
@@ -33,34 +33,49 @@
     <t>4. Verifikacija unesenih podataka</t>
   </si>
   <si>
-    <t>5. Izvjestaj o uspjesnoj verifikaciji</t>
-  </si>
-  <si>
-    <t>i dodjela pristupa</t>
-  </si>
-  <si>
-    <t>6. Napustanje ustanove i obavijest</t>
-  </si>
-  <si>
-    <t>sistema o tome</t>
-  </si>
-  <si>
-    <t>7. Zaprimanje obavijesti o napustanju</t>
-  </si>
-  <si>
-    <t>ustanove</t>
-  </si>
-  <si>
     <t>2. Zahtjev za pristupnim podacima</t>
   </si>
   <si>
     <t>3. Unos pristupnih podataka</t>
   </si>
   <si>
-    <t>Podrazumijevano stanje je da za uposlenika koji se pokusava prijaviti sa</t>
-  </si>
-  <si>
-    <t>RFID karticom vec postoji kreiran racun u bazi podataka od strane admina</t>
+    <t>i obavjestavanje administratora o tome</t>
+  </si>
+  <si>
+    <t>5. Potvrda o prijemu informacija i</t>
+  </si>
+  <si>
+    <t>dodjela pristupa</t>
+  </si>
+  <si>
+    <t>6. Izvjestaj o uspjesnoj verifikaciji</t>
+  </si>
+  <si>
+    <t>se salje na interface</t>
+  </si>
+  <si>
+    <t>8. Potvrda o ulasku u ustanovu</t>
+  </si>
+  <si>
+    <t>9. Prijava napustanja ustanove</t>
+  </si>
+  <si>
+    <t>10. Kreiranje izvjestaja o napustanju</t>
+  </si>
+  <si>
+    <t>11. Zaprimanje izvjestaja</t>
+  </si>
+  <si>
+    <t>o napustanju ustanove</t>
+  </si>
+  <si>
+    <t>ustanove i slanje administratoru</t>
+  </si>
+  <si>
+    <t>i dodjeli pristupa</t>
+  </si>
+  <si>
+    <t>7. Ulazak(boravak) u ustanovu(i)</t>
   </si>
 </sst>
 </file>
@@ -198,8 +213,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -218,33 +260,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,291 +558,301 @@
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
     <col min="17" max="17" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="1" t="s">
+      <c r="E1" s="11"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="3"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="12"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="6"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="15"/>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="12"/>
-      <c r="K3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="3"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="6"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
     </row>
     <row r="4" spans="1:17" ht="15.75" thickBot="1">
       <c r="A4" s="7"/>
       <c r="B4" s="8"/>
       <c r="C4" s="9"/>
-      <c r="D4" s="7"/>
+      <c r="D4" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="E4" s="8"/>
       <c r="F4" s="9"/>
       <c r="G4" s="7"/>
       <c r="H4" s="8"/>
       <c r="I4" s="9"/>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="5"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="6"/>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="A5" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="12"/>
-    </row>
-    <row r="6" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A6" s="14"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="15"/>
-    </row>
-    <row r="7" spans="1:17">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="12"/>
-    </row>
-    <row r="8" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A8" s="14"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="15"/>
-    </row>
-    <row r="9" spans="1:17">
-      <c r="A9" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="12"/>
-    </row>
-    <row r="10" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A10" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="15"/>
-    </row>
-    <row r="11" spans="1:17">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="12"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A12" s="14"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="15"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:17">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="12"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A14" s="14"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="15"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="10"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="12"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A16" s="14"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="15"/>
+      <c r="A16" s="1"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="12"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="6"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A18" s="14"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="15"/>
+      <c r="A18" s="1"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="12"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="6"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A20" s="14"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="15"/>
+      <c r="A20" s="1"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="12"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="6"/>
     </row>
     <row r="22" spans="1:9" ht="15.75" thickBot="1">
       <c r="A22" s="7"/>
@@ -840,7 +866,54 @@
       <c r="I22" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="65">
+  <mergeCells count="63">
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="D1:F2"/>
+    <mergeCell ref="G1:I2"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="D6:F6"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="D19:F19"/>
     <mergeCell ref="G19:I19"/>
@@ -857,55 +930,6 @@
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="G10:I10"/>
     <mergeCell ref="D12:F12"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D1:F2"/>
-    <mergeCell ref="G1:I2"/>
-    <mergeCell ref="K3:Q3"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A3:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>